<commit_message>
day 3 updates: tidy data!!
</commit_message>
<xml_diff>
--- a/data/LotR_Words.xlsx
+++ b/data/LotR_Words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffgoldsmith/Desktop/crash_course/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{37D352F5-E30A-BD43-A7A0-3CD8E155F14A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FDD1B080-6006-AE4F-A6FE-E2929FA40DCE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16000" windowHeight="11540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,6 +197,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -206,8 +208,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,28 +491,28 @@
   <dimension ref="B1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="222" zoomScaleNormal="222" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="F2" s="11" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="J2" s="11" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="15"/>
+      <c r="J2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -552,7 +552,7 @@
       <c r="C4" s="6">
         <v>1229</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>971</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -581,7 +581,7 @@
       <c r="C5" s="6">
         <v>14</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="11">
         <v>3644</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -610,7 +610,7 @@
       <c r="C6" s="9">
         <v>0</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>1995</v>
       </c>
       <c r="F6" s="8" t="s">

</xml_diff>